<commit_message>
CHANGES: - added personal evaluations - added radar charts
</commit_message>
<xml_diff>
--- a/design_IPT/confronto_IPT_Moovit.xlsx
+++ b/design_IPT/confronto_IPT_Moovit.xlsx
@@ -8,14 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennycaruso/Desktop/IPT/design_IPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512D6C43-332B-6E4A-82E3-DED3DA676411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3CDFAC-9151-084E-9D13-C6D6D66849BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0B05A318-767F-8B45-8477-4D31F2A139B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$E$68:$E$74</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$E$68:$E$74</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$E$68:$E$74</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$E$68:$E$74</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$E$68:$E$74</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$E$68:$E$74</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$68:$E$74</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$68:$A$74</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$68:$B$74</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$68:$C$74</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$D$68:$D$74</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$68:$E$74</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -389,9 +431,8 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -401,14 +442,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,6 +467,2167 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Moovit</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="filled"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$68:$B$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.8928571428571429</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5357142857142857</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9559-CD4C-BEF7-A2DF4BDDC384}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$68:$C$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9559-CD4C-BEF7-A2DF4BDDC384}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$68:$D$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9559-CD4C-BEF7-A2DF4BDDC384}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$68:$E$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9559-CD4C-BEF7-A2DF4BDDC384}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="832343264"/>
+        <c:axId val="295017552"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="832343264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="295017552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="295017552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="832343264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>IPT</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="filled"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$68:$F$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.8214285714285714</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6785714285714286</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8214285714285714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-35A1-304A-93F2-01F33FD1237A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$68:$G$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-35A1-304A-93F2-01F33FD1237A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$68:$H$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-35A1-304A-93F2-01F33FD1237A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Adeguatezza al compito (suitability for the task) </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Auto-descrizione (self-descriptiveness) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Conformità alle aspettative dell’utente (conformity with user expectations) </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adeguatezza all’apprendimento (suitability for learning) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Controllabilità (controllability) </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tolleranza verso gli errori (error-tolerance) </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adeguatezza all’individualizzazione (suitability for individualization) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$68:$I$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-35A1-304A-93F2-01F33FD1237A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="330495760"/>
+        <c:axId val="330497408"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="330495760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="330497408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="330497408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="330495760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>538480</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>66040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>207066</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>138044</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9C16642-4D87-4346-8B48-E8084DD157BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{442228C4-B7DE-2146-9254-B06387AEB80D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83634C8-7FE7-F549-BB2F-C3DE6BC80852}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" zoomScaleNormal="236" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="194" workbookViewId="0">
+      <selection activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,24 +2939,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +2987,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -796,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -813,7 +3016,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -825,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -842,7 +3045,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -854,7 +3057,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -871,7 +3074,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -883,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -900,7 +3103,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -912,7 +3115,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -929,7 +3132,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -941,7 +3144,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -958,7 +3161,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -970,7 +3173,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -983,22 +3186,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -1010,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1027,7 +3230,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -1039,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -1056,7 +3259,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -1068,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -1085,7 +3288,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -1097,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1114,7 +3317,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1126,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -1143,7 +3346,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -1155,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -1172,7 +3375,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -1184,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
@@ -1197,22 +3400,22 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -1224,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
@@ -1241,7 +3444,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -1253,7 +3456,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1270,7 +3473,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -1282,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
@@ -1299,7 +3502,7 @@
         <v>30</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -1311,7 +3514,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
@@ -1328,7 +3531,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1340,7 +3543,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -1357,7 +3560,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -1369,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -1386,7 +3589,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -1398,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
@@ -1415,7 +3618,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1427,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G26" s="1">
         <v>0</v>
@@ -1444,7 +3647,7 @@
         <v>35</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -1456,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G27" s="1">
         <v>0</v>
@@ -1473,7 +3676,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -1485,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
@@ -1498,22 +3701,22 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
@@ -1525,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G30" s="1">
         <v>0</v>
@@ -1542,7 +3745,7 @@
         <v>38</v>
       </c>
       <c r="B31" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -1554,7 +3757,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
@@ -1571,7 +3774,7 @@
         <v>39</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -1583,7 +3786,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
@@ -1600,7 +3803,7 @@
         <v>40</v>
       </c>
       <c r="B33" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
@@ -1612,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
@@ -1629,7 +3832,7 @@
         <v>41</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
@@ -1641,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
@@ -1658,7 +3861,7 @@
         <v>42</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -1670,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G35" s="1">
         <v>0</v>
@@ -1687,7 +3890,7 @@
         <v>43</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C36" s="1">
         <v>0</v>
@@ -1699,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G36" s="1">
         <v>0</v>
@@ -1712,22 +3915,22 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
@@ -1739,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
@@ -1756,7 +3959,7 @@
         <v>45</v>
       </c>
       <c r="B39" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
@@ -1768,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
@@ -1785,7 +3988,7 @@
         <v>46</v>
       </c>
       <c r="B40" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
@@ -1797,7 +4000,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
@@ -1814,7 +4017,7 @@
         <v>48</v>
       </c>
       <c r="B41" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C41" s="1">
         <v>0</v>
@@ -1826,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
@@ -1855,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
@@ -1901,7 +4104,7 @@
         <v>50</v>
       </c>
       <c r="B44" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1">
         <v>0</v>
@@ -1913,7 +4116,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
@@ -1942,7 +4145,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
@@ -1955,22 +4158,22 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B47" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
@@ -1982,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -1999,7 +4202,7 @@
         <v>53</v>
       </c>
       <c r="B48" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C48" s="1">
         <v>0</v>
@@ -2011,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -2028,7 +4231,7 @@
         <v>54</v>
       </c>
       <c r="B49" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C49" s="1">
         <v>0</v>
@@ -2040,7 +4243,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
@@ -2057,7 +4260,7 @@
         <v>55</v>
       </c>
       <c r="B50" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1">
         <v>0</v>
@@ -2069,7 +4272,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
@@ -2086,7 +4289,7 @@
         <v>56</v>
       </c>
       <c r="B51" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
@@ -2098,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G51" s="1">
         <v>0</v>
@@ -2115,7 +4318,7 @@
         <v>57</v>
       </c>
       <c r="B52" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C52" s="1">
         <v>0</v>
@@ -2127,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G52" s="1">
         <v>0</v>
@@ -2144,7 +4347,7 @@
         <v>58</v>
       </c>
       <c r="B53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
@@ -2156,7 +4359,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G53" s="1">
         <v>0</v>
@@ -2173,7 +4376,7 @@
         <v>59</v>
       </c>
       <c r="B54" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
@@ -2185,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G54" s="1">
         <v>0</v>
@@ -2202,7 +4405,7 @@
         <v>60</v>
       </c>
       <c r="B55" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
@@ -2214,7 +4417,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G55" s="1">
         <v>0</v>
@@ -2231,7 +4434,7 @@
         <v>61</v>
       </c>
       <c r="B56" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C56" s="1">
         <v>0</v>
@@ -2243,7 +4446,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G56" s="1">
         <v>0</v>
@@ -2256,15 +4459,15 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -2283,7 +4486,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G58" s="1">
         <v>0</v>
@@ -2312,7 +4515,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
@@ -2358,7 +4561,7 @@
         <v>65</v>
       </c>
       <c r="B61" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1">
         <v>0</v>
@@ -2370,7 +4573,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G61" s="1">
         <v>0</v>
@@ -2399,7 +4602,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="1">
         <v>0</v>
@@ -2445,7 +4648,7 @@
         <v>68</v>
       </c>
       <c r="B64" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C64" s="1">
         <v>0</v>
@@ -2457,7 +4660,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G64" s="1">
         <v>0</v>
@@ -2502,184 +4705,196 @@
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="3" t="s">
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="6"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="4">
         <f>AVERAGE(B3:E9)</f>
-        <v>0</v>
-      </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="3">
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="4">
         <f>AVERAGE(F3:I9)</f>
-        <v>0</v>
-      </c>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="5"/>
+        <v>0.8214285714285714</v>
+      </c>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="6"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="4">
         <f>AVERAGE(B11:E17)</f>
-        <v>0</v>
-      </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="3">
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="4">
         <f>AVERAGE(F11:I17)</f>
-        <v>0</v>
-      </c>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="5"/>
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="6"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="4">
         <f>AVERAGE(B19:E28)</f>
-        <v>0</v>
-      </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="4">
         <f>AVERAGE(F19:I28)</f>
-        <v>0</v>
-      </c>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="5"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="4">
         <f>AVERAGE(B30:E36)</f>
-        <v>0</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="4">
         <f>AVERAGE(F30:I36)</f>
-        <v>0</v>
-      </c>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="5"/>
+        <v>0.8214285714285714</v>
+      </c>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="6"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="4">
         <f>AVERAGE(B38:E45)</f>
-        <v>0</v>
-      </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="4">
         <f>AVERAGE(F38:I45)</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="5"/>
+        <v>0.71875</v>
+      </c>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="6"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="4">
         <f>AVERAGE(B47:E56)</f>
-        <v>0</v>
-      </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="4">
         <f>AVERAGE(F47:I56)</f>
-        <v>0</v>
-      </c>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="6"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="4">
         <f>AVERAGE(B58:E65)</f>
-        <v>0</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="4">
         <f>AVERAGE(F58:I65)</f>
-        <v>0</v>
-      </c>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="5"/>
+        <v>0.4375</v>
+      </c>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="6"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="9"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="3"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="4">
         <f>AVERAGE(B68:E74)</f>
-        <v>0</v>
-      </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="3">
+        <v>0.62104591836734702</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="4">
         <f>AVERAGE(F68:I74)</f>
-        <v>0</v>
-      </c>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="5"/>
+        <v>0.74323979591836731</v>
+      </c>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A46:I46"/>
+    <mergeCell ref="A57:I57"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:I67"/>
     <mergeCell ref="F76:I76"/>
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="B74:E74"/>
@@ -2696,19 +4911,8 @@
     <mergeCell ref="B70:E70"/>
     <mergeCell ref="B71:E71"/>
     <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A46:I46"/>
-    <mergeCell ref="A57:I57"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHANGES: - renamed some of the cells according with the Evaluation Guidelines - removed a duplicate cell
</commit_message>
<xml_diff>
--- a/design_IPT/confronto_IPT_Moovit.xlsx
+++ b/design_IPT/confronto_IPT_Moovit.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominickferraro/eclipse-workspace/IPT/design_IPT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennycaruso/Desktop/IPT/design_IPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805B13DB-5DE2-B846-8207-7B37C585958F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0033004A-D244-9548-92E1-51596FD0205E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{0B05A318-767F-8B45-8477-4D31F2A139B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0B05A318-767F-8B45-8477-4D31F2A139B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Confronto_IPT_Moovit_Sheet_1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Denny</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Manualistica minima</t>
   </si>
   <si>
-    <t>Formati descritti</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Guida per l’utente</t>
   </si>
   <si>
@@ -141,12 +138,6 @@
     <t xml:space="preserve"> Messaggi in posizione appropriata</t>
   </si>
   <si>
-    <t xml:space="preserve"> Input in posizione attesa </t>
-  </si>
-  <si>
-    <t>Stile coerente dei messaggi e permettergli di modificarla</t>
-  </si>
-  <si>
     <t>Linguaggio familiare</t>
   </si>
   <si>
@@ -213,15 +204,6 @@
     <t xml:space="preserve">Assistenza per il recupero </t>
   </si>
   <si>
-    <t>Minimo sforzo di recupero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recupero differibile </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Recupero automatico modificabile</t>
-  </si>
-  <si>
     <t>Assistenza all’utente</t>
   </si>
   <si>
@@ -243,9 +225,6 @@
     <t xml:space="preserve">Ripristinabilità dei valori precedenti </t>
   </si>
   <si>
-    <t>Personalizzazione dei tempi di risposta.</t>
-  </si>
-  <si>
     <t>Scelta di rappresentazioni alternative</t>
   </si>
   <si>
@@ -259,13 +238,31 @@
   </si>
   <si>
     <t>Media complessiva:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Input in posizione appropriata </t>
+  </si>
+  <si>
+    <t>Stile coerente dei messaggi</t>
+  </si>
+  <si>
+    <t>Minimo sforzo di correzione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correzione differibile </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Correzione automatica modificabile</t>
+  </si>
+  <si>
+    <t>Personalizzazione dei tempi di risposta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +274,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -386,12 +391,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -403,15 +424,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,7 +445,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -492,7 +507,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -516,7 +531,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -545,7 +560,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$68:$B$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$B$67:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -553,13 +568,13 @@
                   <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1071428571428572</c:v>
+                  <c:v>1.0833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5249999999999999</c:v>
+                  <c:v>1.4750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>1.4285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.25</c:v>
@@ -593,7 +608,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -622,7 +637,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$68:$C$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$C$67:$C$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -649,7 +664,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -678,7 +693,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$68:$D$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$D$67:$D$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -705,7 +720,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -734,7 +749,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$68:$E$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$E$67:$E$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -813,7 +828,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="295017552"/>
@@ -872,7 +887,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="832343264"/>
@@ -920,7 +935,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -934,7 +949,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -996,7 +1011,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1020,7 +1035,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1049,7 +1064,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$68:$F$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$F$67:$F$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1057,7 +1072,7 @@
                   <c:v>1.6785714285714286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4285714285714286</c:v>
+                  <c:v>1.4583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.85</c:v>
@@ -1097,7 +1112,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1126,7 +1141,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$68:$G$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$G$67:$G$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1153,7 +1168,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1182,7 +1197,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$68:$H$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$H$67:$H$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1209,7 +1224,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$68:$A$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$A$67:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1238,7 +1253,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$68:$I$74</c:f>
+              <c:f>Confronto_IPT_Moovit_Sheet_1!$I$67:$I$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1303,7 +1318,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="330497408"/>
@@ -1362,7 +1377,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="330495760"/>
@@ -1410,7 +1425,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2517,13 +2532,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>538480</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>66040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>207066</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>138044</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2553,13 +2568,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2589,7 +2604,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2885,10 +2900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83634C8-7FE7-F549-BB2F-C3DE6BC80852}">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="194" workbookViewId="0">
-      <selection activeCell="S95" sqref="S95"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="194" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2897,24 +2912,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3144,19 +3159,19 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -3301,7 +3316,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
@@ -3310,70 +3325,70 @@
         <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
         <v>2</v>
       </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>3</v>
-      </c>
       <c r="I16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>2</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -3402,7 +3417,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -3437,13 +3452,13 @@
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
@@ -3460,19 +3475,19 @@
         <v>30</v>
       </c>
       <c r="B22" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
@@ -3489,7 +3504,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -3501,13 +3516,13 @@
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -3518,7 +3533,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -3530,7 +3545,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -3553,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -3565,7 +3580,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -3573,16 +3588,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
       </c>
       <c r="D26" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -3594,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -3602,76 +3617,76 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B27" s="1">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1">
         <v>2</v>
       </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <v>2</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <v>4</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <v>3</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="1">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1">
-        <v>3</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1">
-        <v>4</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
-        <v>4</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="7"/>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1">
         <v>4</v>
@@ -3680,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -3700,22 +3715,22 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
       </c>
       <c r="D31" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
       </c>
       <c r="F31" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
@@ -3729,10 +3744,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -3750,7 +3765,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I32" s="1">
         <v>0</v>
@@ -3758,28 +3773,28 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
       </c>
       <c r="H33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -3787,16 +3802,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -3808,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
@@ -3816,16 +3831,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
       </c>
       <c r="D35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -3837,55 +3852,55 @@
         <v>0</v>
       </c>
       <c r="H35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="1">
-        <v>3</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1">
-        <v>3</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>3</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>3</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0</v>
-      </c>
+      <c r="A36" s="11"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="7"/>
+      <c r="A37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>4</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1">
         <v>4</v>
@@ -3914,16 +3929,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
       </c>
       <c r="D39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -3935,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I39" s="1">
         <v>0</v>
@@ -3943,22 +3958,22 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
       </c>
       <c r="D40" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
@@ -3972,16 +3987,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C41" s="1">
         <v>0</v>
       </c>
       <c r="D41" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -4001,7 +4016,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -4010,19 +4025,19 @@
         <v>0</v>
       </c>
       <c r="D42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
       </c>
       <c r="H42" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42" s="1">
         <v>0</v>
@@ -4030,28 +4045,28 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B43" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C43" s="1">
         <v>0</v>
       </c>
       <c r="D43" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
       </c>
       <c r="H43" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
@@ -4059,85 +4074,85 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B44" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C44" s="1">
         <v>0</v>
       </c>
       <c r="D44" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="1">
-        <v>0</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-      <c r="F45" s="1">
-        <v>2</v>
-      </c>
-      <c r="G45" s="1">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1">
-        <v>1</v>
-      </c>
-      <c r="I45" s="1">
-        <v>0</v>
-      </c>
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="13"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="7"/>
+      <c r="A46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>4</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>4</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
       </c>
       <c r="D47" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -4157,7 +4172,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -4186,7 +4201,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1">
         <v>4</v>
@@ -4215,28 +4230,28 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="1">
         <v>0</v>
       </c>
       <c r="D50" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
       </c>
       <c r="H50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I50" s="1">
         <v>0</v>
@@ -4244,7 +4259,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1">
         <v>2</v>
@@ -4273,16 +4288,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
         <v>2</v>
-      </c>
-      <c r="C52" s="1">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -4302,16 +4317,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
         <v>1</v>
-      </c>
-      <c r="C53" s="1">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1">
-        <v>2</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -4331,28 +4346,28 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
         <v>2</v>
       </c>
-      <c r="C54" s="1">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="1">
-        <v>3</v>
-      </c>
       <c r="G54" s="1">
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I54" s="1">
         <v>0</v>
@@ -4360,7 +4375,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B55" s="1">
         <v>3</v>
@@ -4388,48 +4403,48 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="1">
-        <v>3</v>
-      </c>
-      <c r="C56" s="1">
-        <v>0</v>
-      </c>
-      <c r="D56" s="1">
-        <v>3</v>
-      </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-      <c r="F56" s="1">
-        <v>2</v>
-      </c>
-      <c r="G56" s="1">
-        <v>0</v>
-      </c>
-      <c r="H56" s="1">
-        <v>2</v>
-      </c>
-      <c r="I56" s="1">
-        <v>0</v>
-      </c>
+      <c r="A56" s="11"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="7"/>
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>3</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -4444,7 +4459,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G58" s="1">
         <v>0</v>
@@ -4458,7 +4473,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
@@ -4473,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
@@ -4487,28 +4502,28 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
       </c>
       <c r="D60" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I60" s="1">
         <v>0</v>
@@ -4516,28 +4531,28 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B61" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C61" s="1">
         <v>0</v>
       </c>
       <c r="D61" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G61" s="1">
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
@@ -4545,7 +4560,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -4574,7 +4589,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
@@ -4603,7 +4618,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1">
         <v>2</v>
@@ -4630,244 +4645,215 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="1">
-        <v>0</v>
-      </c>
-      <c r="C65" s="1">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1">
-        <v>0</v>
-      </c>
-      <c r="F65" s="1">
-        <v>0</v>
-      </c>
-      <c r="G65" s="1">
-        <v>0</v>
-      </c>
-      <c r="H65" s="1">
-        <v>0</v>
-      </c>
-      <c r="I65" s="1">
-        <v>0</v>
-      </c>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="8"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="B67" s="11">
+        <f>AVERAGE(B3:E9)</f>
+        <v>1.75</v>
+      </c>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="11">
+        <f>AVERAGE(F3:I9)</f>
+        <v>1.6785714285714286</v>
+      </c>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="13"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" s="5">
-        <f>AVERAGE(B3:E9)</f>
-        <v>1.75</v>
-      </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="5">
-        <f>AVERAGE(F3:I9)</f>
-        <v>1.6785714285714286</v>
-      </c>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="B68" s="11">
+        <f>AVERAGE(B11:E16)</f>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="11">
+        <f>AVERAGE(F11:I16)</f>
+        <v>1.4583333333333333</v>
+      </c>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="13"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B69" s="5">
-        <f>AVERAGE(B11:E17)</f>
-        <v>1.1071428571428572</v>
-      </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="5">
-        <f>AVERAGE(F11:I17)</f>
-        <v>1.4285714285714286</v>
-      </c>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B69" s="11">
+        <f>AVERAGE(B18:E27)</f>
+        <v>1.4750000000000001</v>
+      </c>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="11">
+        <f>AVERAGE(F18:I27)</f>
+        <v>1.85</v>
+      </c>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="13"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B70" s="5">
-        <f>AVERAGE(B19:E28)</f>
-        <v>1.5249999999999999</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="5">
-        <f>AVERAGE(F19:I28)</f>
-        <v>1.85</v>
-      </c>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="B70" s="11">
+        <f>AVERAGE(B29:E35)</f>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="11">
+        <f>AVERAGE(F29:I35)</f>
+        <v>1.6428571428571428</v>
+      </c>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="13"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="5">
-        <f>AVERAGE(B30:E36)</f>
-        <v>1.5</v>
-      </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="5">
-        <f>AVERAGE(F30:I36)</f>
-        <v>1.6428571428571428</v>
-      </c>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="B71" s="11">
+        <f>AVERAGE(B37:E44)</f>
+        <v>1.25</v>
+      </c>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="11">
+        <f>AVERAGE(F37:I44)</f>
+        <v>1.40625</v>
+      </c>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="13"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B72" s="5">
-        <f>AVERAGE(B38:E45)</f>
-        <v>1.25</v>
-      </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="5">
-        <f>AVERAGE(F38:I45)</f>
-        <v>1.40625</v>
-      </c>
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="B72" s="11">
+        <f>AVERAGE(B46:E55)</f>
+        <v>1.35</v>
+      </c>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="11">
+        <f>AVERAGE(F46:I55)</f>
+        <v>1.6</v>
+      </c>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="13"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="5">
-        <f>AVERAGE(B47:E56)</f>
-        <v>1.35</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="5">
-        <f>AVERAGE(F47:I56)</f>
-        <v>1.6</v>
-      </c>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="B73" s="11">
+        <f>AVERAGE(B57:E64)</f>
+        <v>0.25</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="11">
+        <f>AVERAGE(F57:I64)</f>
+        <v>0.65625</v>
+      </c>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="13"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B74" s="5">
-        <f>AVERAGE(B58:E65)</f>
-        <v>0.25</v>
-      </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="5">
-        <f>AVERAGE(F58:I65)</f>
-        <v>0.65625</v>
-      </c>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="7"/>
+      <c r="A74" s="11"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="3"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" s="5">
-        <f>AVERAGE(B68:E74)</f>
-        <v>1.2474489795918369</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="5">
-        <f>AVERAGE(F68:I74)</f>
-        <v>1.4660714285714285</v>
-      </c>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="7"/>
+      <c r="A75" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="11">
+        <f>AVERAGE(B67:E73)</f>
+        <v>1.2267006802721088</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="11">
+        <f>AVERAGE(F67:I73)</f>
+        <v>1.4703231292517007</v>
+      </c>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="F67:I67"/>
     <mergeCell ref="F68:I68"/>
     <mergeCell ref="F69:I69"/>
     <mergeCell ref="F70:I70"/>
     <mergeCell ref="F71:I71"/>
     <mergeCell ref="F72:I72"/>
     <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="B67:E67"/>
     <mergeCell ref="B68:E68"/>
     <mergeCell ref="B69:E69"/>
     <mergeCell ref="B70:E70"/>
     <mergeCell ref="B71:E71"/>
     <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A46:I46"/>
-    <mergeCell ref="A57:I57"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:I66"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A17:I17"/>
     <mergeCell ref="A10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update radar chart and RAD relative import
</commit_message>
<xml_diff>
--- a/design_IPT/confronto_IPT_Moovit.xlsx
+++ b/design_IPT/confronto_IPT_Moovit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maax\vscode-workspace\IPT\design_IPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennycaruso/Desktop/IPT/design_IPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A48704-A8A0-4CE5-A2EA-CA4FE5932D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AE00C4-ECC3-384B-A1CA-969B899ED929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B05A318-767F-8B45-8477-4D31F2A139B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0B05A318-767F-8B45-8477-4D31F2A139B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Confronto_IPT_Moovit_Sheet_1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -429,24 +435,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +465,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -527,7 +527,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -848,7 +848,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="295017552"/>
@@ -907,7 +907,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="832343264"/>
@@ -955,7 +955,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -969,7 +969,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1031,7 +1031,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1101,13 +1101,13 @@
                   <c:v>3.1785714285714284</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.59375</c:v>
+                  <c:v>2.53125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.15</c:v>
+                  <c:v>3.05</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.09375</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1338,7 +1338,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="330497408"/>
@@ -1397,7 +1397,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="330495760"/>
@@ -1445,7 +1445,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2624,7 +2624,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2922,34 +2922,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83634C8-7FE7-F549-BB2F-C3DE6BC80852}">
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="125" zoomScaleNormal="194" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" zoomScaleNormal="194" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69:I69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="69.19921875" customWidth="1"/>
+    <col min="1" max="1" width="69.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -3179,18 +3179,18 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -3365,18 +3365,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -3667,18 +3667,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="16"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -3881,18 +3881,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="16"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="F39" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" s="1">
         <v>2</v>
@@ -3979,7 +3979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>4</v>
       </c>
       <c r="F44" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
@@ -4124,18 +4124,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="16"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="10"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G48" s="1">
         <v>4</v>
@@ -4222,7 +4222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G53" s="1">
         <v>3</v>
@@ -4367,7 +4367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>71</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>72</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>3</v>
       </c>
       <c r="F55" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="1">
         <v>1</v>
@@ -4425,18 +4425,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="14"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="16"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G60" s="1">
         <v>2</v>
@@ -4552,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G64" s="1">
         <v>1</v>
@@ -4668,188 +4668,200 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="9" t="s">
+      <c r="B66" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="11"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="13"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B67" s="14">
+      <c r="B67" s="8">
         <f>AVERAGE(B3:E9)</f>
         <v>3.4285714285714284</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="14">
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="8">
         <f>AVERAGE(F3:I9)</f>
         <v>3.4285714285714284</v>
       </c>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="16"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="10"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="14">
+      <c r="B68" s="8">
         <f>AVERAGE(B11:E16)</f>
         <v>2.0833333333333335</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="14">
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="8">
         <f>AVERAGE(F11:I16)</f>
         <v>2.75</v>
       </c>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15"/>
-      <c r="I68" s="16"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="10"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B69" s="14">
+      <c r="B69" s="8">
         <f>AVERAGE(B18:E27)</f>
         <v>3</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="14">
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="8">
         <f>AVERAGE(F18:I27)</f>
         <v>3.7749999999999999</v>
       </c>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="16"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="10"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="14">
+      <c r="B70" s="8">
         <f>AVERAGE(B29:E35)</f>
         <v>2.8214285714285716</v>
       </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="14">
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="8">
         <f>AVERAGE(F29:I35)</f>
         <v>3.1785714285714284</v>
       </c>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="16"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="10"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B71" s="8">
         <f>AVERAGE(B37:E44)</f>
         <v>2.4375</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="14">
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="8">
         <f>AVERAGE(F37:I44)</f>
-        <v>2.59375</v>
-      </c>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15"/>
-      <c r="I71" s="16"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.53125</v>
+      </c>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="10"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="14">
+      <c r="B72" s="8">
         <f>AVERAGE(B46:E55)</f>
         <v>2.4750000000000001</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="14">
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="8">
         <f>AVERAGE(F46:I55)</f>
-        <v>3.15</v>
-      </c>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="16"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3.05</v>
+      </c>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B73" s="14">
+      <c r="B73" s="8">
         <f>AVERAGE(B57:E64)</f>
         <v>0.40625</v>
       </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="14">
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="8">
         <f>AVERAGE(F57:I64)</f>
-        <v>1.09375</v>
-      </c>
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
-      <c r="I73" s="16"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="15"/>
+        <v>0.875</v>
+      </c>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="10"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="8"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="3"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B75" s="14">
+      <c r="B75" s="8">
         <f>AVERAGE(B67:E73)</f>
         <v>2.3788690476190477</v>
       </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="14">
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="8">
         <f>AVERAGE(F67:I73)</f>
-        <v>2.8528061224489796</v>
-      </c>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
-      <c r="I75" s="16"/>
+        <v>2.7983418367346937</v>
+      </c>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:I66"/>
     <mergeCell ref="F75:I75"/>
     <mergeCell ref="A74:F74"/>
     <mergeCell ref="B73:E73"/>
@@ -4866,18 +4878,6 @@
     <mergeCell ref="B69:E69"/>
     <mergeCell ref="B70:E70"/>
     <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A56:I56"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>